<commit_message>
Create more test cases
</commit_message>
<xml_diff>
--- a/test_cases/combined production with byproduct - expected case.xlsx
+++ b/test_cases/combined production with byproduct - expected case.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">meta!$A$1:$B$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">quantitative!$A$1:$U$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">quantitative!$A$1:$U$7</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="90">
   <si>
     <t>access restricted</t>
   </si>
@@ -190,6 +190,9 @@
     <t>byproduct</t>
   </si>
   <si>
+    <t>from technosphere</t>
+  </si>
+  <si>
     <t>from environment</t>
   </si>
   <si>
@@ -199,12 +202,18 @@
     <t>exchange_04</t>
   </si>
   <si>
+    <t>exchange_05</t>
+  </si>
+  <si>
     <t>parameter_01</t>
   </si>
   <si>
     <t>heat</t>
   </si>
   <si>
+    <t>coal</t>
+  </si>
+  <si>
     <t>carbon dioxide, fossil</t>
   </si>
   <si>
@@ -290,21 +299,6 @@
   </si>
   <si>
     <t>combined production with byproduct - expected case</t>
-  </si>
-  <si>
-    <t>gold</t>
-  </si>
-  <si>
-    <t>silver</t>
-  </si>
-  <si>
-    <t>gold powder</t>
-  </si>
-  <si>
-    <t>silver powder</t>
-  </si>
-  <si>
-    <t>sludge</t>
   </si>
 </sst>
 </file>
@@ -634,7 +628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
@@ -657,7 +651,7 @@
         <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -681,7 +675,7 @@
         <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -749,10 +743,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U14"/>
+  <dimension ref="A1:U12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -840,19 +834,19 @@
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>87</v>
+        <v>11</v>
       </c>
       <c r="J2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="K2">
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="N2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
@@ -863,22 +857,22 @@
         <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="F3" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="J3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="K3">
         <v>0.3</v>
       </c>
       <c r="L3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="N3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
@@ -889,22 +883,22 @@
         <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F4" t="s">
-        <v>89</v>
+        <v>60</v>
       </c>
       <c r="J4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="K4">
         <v>3</v>
       </c>
       <c r="L4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="N4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
@@ -912,227 +906,220 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F5" t="s">
-        <v>90</v>
-      </c>
-      <c r="J5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" t="s">
         <v>64</v>
+      </c>
+      <c r="K5">
+        <v>5</v>
+      </c>
+      <c r="L5" t="s">
+        <v>71</v>
+      </c>
+      <c r="N5" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
       <c r="E6" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F6" t="s">
-        <v>91</v>
+        <v>61</v>
+      </c>
+      <c r="G6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6" t="s">
+        <v>70</v>
+      </c>
+      <c r="N6" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G7" t="s">
-        <v>60</v>
-      </c>
-      <c r="H7" t="s">
-        <v>61</v>
+        <v>11</v>
+      </c>
+      <c r="J7" t="s">
+        <v>67</v>
       </c>
       <c r="K7">
-        <v>5</v>
+        <v>50000</v>
       </c>
       <c r="L7" t="s">
         <v>68</v>
       </c>
       <c r="N7" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G8" t="s">
-        <v>62</v>
-      </c>
-      <c r="H8" t="s">
-        <v>63</v>
+        <v>59</v>
+      </c>
+      <c r="J8" t="s">
+        <v>67</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>15000</v>
       </c>
       <c r="L8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N8" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>46</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>82</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="J9" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="K9">
-        <v>50000</v>
+        <v>5</v>
       </c>
       <c r="L9" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="N9" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>82</v>
       </c>
       <c r="E10" t="s">
         <v>52</v>
       </c>
       <c r="F10" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="J10" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="K10">
-        <v>15000</v>
+        <v>4</v>
       </c>
       <c r="L10" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="N10" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E11" t="s">
-        <v>6</v>
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>58</v>
       </c>
       <c r="F11" t="s">
-        <v>79</v>
-      </c>
-      <c r="J11" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="K11">
-        <v>5</v>
+        <v>0.11</v>
       </c>
       <c r="L11" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="N11" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>46</v>
       </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
       <c r="C12" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="F12" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="J12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="K12">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="L12" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="N12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" t="s">
         <v>84</v>
       </c>
-      <c r="K13">
-        <v>0.11</v>
-      </c>
-      <c r="L13" t="s">
-        <v>85</v>
-      </c>
-      <c r="N13" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" t="s">
-        <v>82</v>
-      </c>
-      <c r="E14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" t="s">
-        <v>82</v>
-      </c>
-      <c r="J14" t="s">
-        <v>64</v>
-      </c>
-      <c r="K14">
-        <v>11</v>
-      </c>
-      <c r="L14" t="s">
-        <v>85</v>
-      </c>
-      <c r="N14" t="s">
-        <v>81</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U9"/>
+  <autoFilter ref="A1:U7"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>